<commit_message>
11th july run| ||
</commit_message>
<xml_diff>
--- a/webscrapping school/msaces/excel/2025-07-11.xlsx
+++ b/webscrapping school/msaces/excel/2025-07-11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,14 +583,20 @@
       <c r="M2" t="n">
         <v>0</v>
       </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -661,14 +667,20 @@
       <c r="M3" t="n">
         <v>0</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -739,14 +751,20 @@
       <c r="M4" t="n">
         <v>0</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -817,14 +835,20 @@
       <c r="M5" t="n">
         <v>0</v>
       </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -895,14 +919,20 @@
       <c r="M6" t="n">
         <v>0</v>
       </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
@@ -973,14 +1003,20 @@
       <c r="M7" t="n">
         <v>0</v>
       </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
@@ -1051,14 +1087,20 @@
       <c r="M8" t="n">
         <v>0</v>
       </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -1129,14 +1171,20 @@
       <c r="M9" t="n">
         <v>0</v>
       </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
@@ -1207,14 +1255,20 @@
       <c r="M10" t="n">
         <v>0</v>
       </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -1285,14 +1339,20 @@
       <c r="M11" t="n">
         <v>0</v>
       </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
@@ -1363,14 +1423,20 @@
       <c r="M12" t="n">
         <v>0</v>
       </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
@@ -1441,14 +1507,20 @@
       <c r="M13" t="n">
         <v>0</v>
       </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
@@ -1523,14 +1595,20 @@
       <c r="M14" t="n">
         <v>0</v>
       </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0</v>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
@@ -1605,14 +1683,20 @@
       <c r="M15" t="n">
         <v>0</v>
       </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0</v>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
@@ -1683,14 +1767,20 @@
       <c r="M16" t="n">
         <v>0</v>
       </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0</v>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
@@ -1765,14 +1855,20 @@
       <c r="M17" t="n">
         <v>0</v>
       </c>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0</v>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
@@ -1843,14 +1939,20 @@
       <c r="M18" t="n">
         <v>0</v>
       </c>
-      <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0</v>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
@@ -1866,41 +1968,41 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>748322</t>
+          <t>748331</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025.06.25</t>
+          <t>2025.06.24</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>LISBOAGÁS COMERCIALIZAÇÃO, S.A. PT LUSITANIAGÁS COMERCIALIZAÇÃO, S.A. PT SETGÁS COMERCIALIZAÇÃO, S.A. PT TRANSGÁS, S.A.</t>
+          <t>MISTÉRIO DA TERRA S.A.</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.racius.com/setgas-sociedade-de-distribuicao-de-gas-natural-s-a/</t>
+          <t>https://www.racius.com/misterio-da-terra-s-a/</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>502404124</t>
+          <t>509623794</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Avenida Alexandre Herculano, N.º36, R/C Dtº</t>
+          <t>Rua Casal Canas, 14 - 3 A</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2900-205 Setubal</t>
+          <t>2790-204 Carnaxide</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1921,14 +2023,20 @@
       <c r="M19" t="n">
         <v>0</v>
       </c>
-      <c r="N19" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0</v>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
@@ -1944,7 +2052,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>748331</t>
+          <t>748332</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1954,31 +2062,31 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MISTÉRIO DA TERRA S.A.</t>
+          <t>MARWAN BADA UNIPESSOAL LDA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.racius.com/misterio-da-terra-s-a/</t>
+          <t>https://www.racius.com/marwan-bada-unipessoal-lda/</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>509623794</t>
+          <t>518565351</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Rua Casal Canas, 14 - 3 A</t>
+          <t>Avenida 5 de Outubro, Nº 148, 3º G</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2790-204 Carnaxide</t>
+          <t>2900-309 Setubal</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1999,14 +2107,20 @@
       <c r="M20" t="n">
         <v>0</v>
       </c>
-      <c r="N20" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" t="n">
-        <v>0</v>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
@@ -2022,41 +2136,45 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>748332</t>
+          <t>748359</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025.06.24</t>
+          <t>2025.06.25</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MARWAN BADA UNIPESSOAL LDA</t>
+          <t>ENIGMA VIRTUAL, LDA.</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>35</v>
-      </c>
-      <c r="E21" t="inlineStr"/>
+        <v>42</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>INSPYRAL</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.racius.com/marwan-bada-unipessoal-lda/</t>
+          <t>https://www.racius.com/enigma-virtual-lda/</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>518565351</t>
+          <t>508098092</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Avenida 5 de Outubro, Nº 148, 3º G</t>
+          <t>Rua Pedro Homem de Mello, Nº 55, Sala 5.08</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2900-309 Setubal</t>
+          <t>4150-599 Porto</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2077,14 +2195,20 @@
       <c r="M21" t="n">
         <v>0</v>
       </c>
-      <c r="N21" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" t="n">
-        <v>0</v>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
@@ -2100,7 +2224,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>748359</t>
+          <t>748360</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2110,35 +2234,35 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ENIGMA VIRTUAL, LDA.</t>
+          <t>PART CREATIVE STUDIO, LDA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>INSPYRAL</t>
+          <t>O MOTIVO COMUNICAÇÃO</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.racius.com/enigma-virtual-lda/</t>
+          <t>https://www.racius.com/part-creative-studio-lda/</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>508098092</t>
+          <t>517492040</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Rua Pedro Homem de Mello, Nº 55, Sala 5.08</t>
+          <t>Rua Pinto Ferreira, N.º 22, 3.º Andar Direito</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>4150-599 Porto</t>
+          <t>1300-464 Lisboa</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2159,14 +2283,20 @@
       <c r="M22" t="n">
         <v>0</v>
       </c>
-      <c r="N22" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" t="n">
-        <v>0</v>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
@@ -2182,7 +2312,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>748360</t>
+          <t>748370</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2192,35 +2322,35 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PART CREATIVE STUDIO, LDA</t>
+          <t>DESIDERIO &amp; LESLEY - EXPLORAÇÕES DE BARES, LDA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>O MOTIVO COMUNICAÇÃO</t>
+          <t>OURA BAR</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.racius.com/part-creative-studio-lda/</t>
+          <t>https://www.racius.com/desiderio-lesley-exploracoes-de-bares-lda/</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>517492040</t>
+          <t>508401011</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Rua Pinto Ferreira, N.º 22, 3.º Andar Direito</t>
+          <t>Sítio de Vale Serves, Cx Postal 209 Z, Ferreiras</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>1300-464 Lisboa</t>
+          <t>8200-559 Ferreiras</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2241,14 +2371,20 @@
       <c r="M23" t="n">
         <v>0</v>
       </c>
-      <c r="N23" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" t="n">
-        <v>0</v>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
@@ -2264,45 +2400,45 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>748361</t>
+          <t>748388</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025.06.25</t>
+          <t>2025.06.24</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>DIOGO RODRIGUES SEVERIANO</t>
+          <t>GERAÇÃO MCAR UNIPESSOAL LDA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>UZEE</t>
+          <t>GERAÇÃO MCAR</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.racius.com/rodrigues-sousa-diogo-lda/</t>
+          <t>https://www.racius.com/geracao-mcar-unipessoal-lda/</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>500234990</t>
+          <t>517916800</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Rua Zófimo Pedroso, N 63</t>
+          <t>Zona Industrial da Cocanha, Rua Júlio Santos Pereira 20B</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>1950-290 Lisboa</t>
+          <t>5400-570 Santa Cruz/Trindade e Sanjurge</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2323,14 +2459,20 @@
       <c r="M24" t="n">
         <v>0</v>
       </c>
-      <c r="N24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" t="n">
-        <v>0</v>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
@@ -2346,17 +2488,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>748370</t>
+          <t>748392</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025.06.25</t>
+          <t>2025.06.24</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>DESIDERIO &amp; LESLEY - EXPLORAÇÕES DE BARES, LDA</t>
+          <t>GPR GASTRONOMIA DO PRINCIPE REAL, LDA.</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2364,27 +2506,27 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>OURA BAR</t>
+          <t>OCTO (PUS) DOG</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.racius.com/desiderio-lesley-exploracoes-de-bares-lda/</t>
+          <t>https://www.racius.com/gpr-gastronomia-do-principe-real-lda/</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>508401011</t>
+          <t>510698743</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Sítio de Vale Serves, Cx Postal 209 Z, Ferreiras</t>
+          <t>Rua do Loreto, Nº21, R/C</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>8200-559 Ferreiras</t>
+          <t>1200-241 Lisboa</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2405,14 +2547,20 @@
       <c r="M25" t="n">
         <v>0</v>
       </c>
-      <c r="N25" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" t="n">
-        <v>0</v>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
@@ -2428,7 +2576,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>748388</t>
+          <t>748393</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2438,35 +2586,35 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>GERAÇÃO MCAR UNIPESSOAL LDA</t>
+          <t>GPR GASTRONOMIA DO PRINCIPE REAL, LDA.</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>GERAÇÃO MCAR</t>
+          <t>SEA ME DOG</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.racius.com/geracao-mcar-unipessoal-lda/</t>
+          <t>https://www.racius.com/gpr-gastronomia-do-principe-real-lda/</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>517916800</t>
+          <t>510698743</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Zona Industrial da Cocanha, Rua Júlio Santos Pereira 20B</t>
+          <t>Rua do Loreto, Nº21, R/C</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>5400-570 Santa Cruz/Trindade e Sanjurge</t>
+          <t>1200-241 Lisboa</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2487,14 +2635,20 @@
       <c r="M26" t="n">
         <v>0</v>
       </c>
-      <c r="N26" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" t="n">
-        <v>0</v>
-      </c>
-      <c r="P26" t="n">
-        <v>0</v>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
@@ -2510,7 +2664,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>748392</t>
+          <t>748395</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2520,35 +2674,35 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>GPR GASTRONOMIA DO PRINCIPE REAL, LDA.</t>
+          <t>ABEGOARIA COMERCIAL, S.A.</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>OCTO (PUS) DOG</t>
+          <t>CASTELO DAS PIPAS</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.racius.com/gpr-gastronomia-do-principe-real-lda/</t>
+          <t>https://www.racius.com/abegoaria-comercial-s-a/</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>510698743</t>
+          <t>513777172</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Rua do Loreto, Nº21, R/C</t>
+          <t>Rua do Benquerer - Zona Industrial de Mourão</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>1200-241 Lisboa</t>
+          <t>7240-248 Mourão</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2569,14 +2723,20 @@
       <c r="M27" t="n">
         <v>0</v>
       </c>
-      <c r="N27" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" t="n">
-        <v>0</v>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
@@ -2592,45 +2752,45 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>748393</t>
+          <t>748400</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2025.06.24</t>
+          <t>2025.06.25</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>GPR GASTRONOMIA DO PRINCIPE REAL, LDA.</t>
+          <t>SOCIEDAD DE EXPLOTACION DE REDES ELECTRONICAS Y SERVICIOS S.A. SUCURSAL EM PORTUGAL</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>SEA ME DOG</t>
+          <t>SERES CONNECT</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.racius.com/gpr-gastronomia-do-principe-real-lda/</t>
+          <t>https://www.racius.com/sociedad-de-explotacion-de-redes-electronicas-y-servicios-s-a-sucursal-em-portugal/</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>510698743</t>
+          <t>980624550</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Rua do Loreto, Nº21, R/C</t>
+          <t>Av. da Liberdade, 36, 6º</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>1200-241 Lisboa</t>
+          <t>1250-145 Lisboa</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2651,14 +2811,20 @@
       <c r="M28" t="n">
         <v>0</v>
       </c>
-      <c r="N28" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" t="n">
-        <v>0</v>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
@@ -2674,45 +2840,45 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>748395</t>
+          <t>748401</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2025.06.24</t>
+          <t>2025.06.25</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ABEGOARIA COMERCIAL, S.A.</t>
+          <t>SOCIEDAD DE EXPLOTACION DE REDES ELECTRONICAS Y SERVICIOS S.A. SUCURSAL EM PORTUGAL</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>CASTELO DAS PIPAS</t>
+          <t>SERES E-FACTURA</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.racius.com/abegoaria-comercial-s-a/</t>
+          <t>https://www.racius.com/sociedad-de-explotacion-de-redes-electronicas-y-servicios-s-a-sucursal-em-portugal/</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>513777172</t>
+          <t>980624550</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Rua do Benquerer - Zona Industrial de Mourão</t>
+          <t>Av. da Liberdade, 36, 6º</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>7240-248 Mourão</t>
+          <t>1250-145 Lisboa</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2733,14 +2899,20 @@
       <c r="M29" t="n">
         <v>0</v>
       </c>
-      <c r="N29" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" t="n">
-        <v>0</v>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
@@ -2756,7 +2928,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>748400</t>
+          <t>748402</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2772,11 +2944,7 @@
       <c r="D30" t="n">
         <v>9</v>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>SERES CONNECT</t>
-        </is>
-      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
           <t>https://www.racius.com/sociedad-de-explotacion-de-redes-electronicas-y-servicios-s-a-sucursal-em-portugal/</t>
@@ -2815,14 +2983,20 @@
       <c r="M30" t="n">
         <v>0</v>
       </c>
-      <c r="N30" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" t="n">
-        <v>0</v>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
@@ -2838,7 +3012,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>748401</t>
+          <t>748403</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2848,35 +3022,31 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>SOCIEDAD DE EXPLOTACION DE REDES ELECTRONICAS Y SERVICIOS S.A. SUCURSAL EM PORTUGAL</t>
+          <t>WAKAI MD, LDA.</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>9</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>SERES E-FACTURA</t>
-        </is>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.racius.com/sociedad-de-explotacion-de-redes-electronicas-y-servicios-s-a-sucursal-em-portugal/</t>
+          <t>https://www.racius.com/wakai-md-lda/</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>980624550</t>
+          <t>517231581</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Av. da Liberdade, 36, 6º</t>
+          <t>Avenida Praia da Vitória, N.º 12-B</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>1250-145 Lisboa</t>
+          <t>1000-247 Lisboa</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2897,14 +3067,20 @@
       <c r="M31" t="n">
         <v>0</v>
       </c>
-      <c r="N31" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" t="n">
-        <v>0</v>
-      </c>
-      <c r="P31" t="n">
-        <v>0</v>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
@@ -2920,7 +3096,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>748402</t>
+          <t>748405</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2930,31 +3106,35 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>SOCIEDAD DE EXPLOTACION DE REDES ELECTRONICAS Y SERVICIOS S.A. SUCURSAL EM PORTUGAL</t>
+          <t>FÓRMULAS &amp; DOUTRINAS, LDA</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>9</v>
-      </c>
-      <c r="E32" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>BRITWELL CLINIC</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.racius.com/sociedad-de-explotacion-de-redes-electronicas-y-servicios-s-a-sucursal-em-portugal/</t>
+          <t>https://www.racius.com/formulas-doutrinas-lda/</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>980624550</t>
+          <t>517971135</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Av. da Liberdade, 36, 6º</t>
+          <t>Rua António Nobre, Nº 1D, 3º Dtº</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>1250-145 Lisboa</t>
+          <t>2800-260 Cacilhas</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2975,14 +3155,20 @@
       <c r="M32" t="n">
         <v>0</v>
       </c>
-      <c r="N32" t="n">
-        <v>0</v>
-      </c>
-      <c r="O32" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" t="n">
-        <v>0</v>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
@@ -2998,7 +3184,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>748403</t>
+          <t>748409</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3008,31 +3194,35 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>WAKAI MD, LDA.</t>
+          <t>ZERO DOSAGE, LDA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>10</v>
-      </c>
-      <c r="E33" t="inlineStr"/>
+        <v>33</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>ZERO DOSAGE</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.racius.com/wakai-md-lda/</t>
+          <t>https://www.racius.com/zero-dosage-lda/</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>517231581</t>
+          <t>518764230</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Avenida Praia da Vitória, N.º 12-B</t>
+          <t>Rua Correia de Sá, Nº 349, Casa 7</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>1000-247 Lisboa</t>
+          <t>4150-229 Lordelo do Ouro</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -3053,14 +3243,20 @@
       <c r="M33" t="n">
         <v>0</v>
       </c>
-      <c r="N33" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" t="n">
-        <v>0</v>
-      </c>
-      <c r="P33" t="n">
-        <v>0</v>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
@@ -3076,7 +3272,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>748405</t>
+          <t>748413</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3086,7 +3282,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>FÓRMULAS &amp; DOUTRINAS, LDA</t>
+          <t>TOPPERFORMANCE, LDA</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -3094,27 +3290,27 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>BRITWELL CLINIC</t>
+          <t>SIMPLIFICAMENTE</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.racius.com/formulas-doutrinas-lda/</t>
+          <t>https://www.racius.com/topperformance-lda/</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>517971135</t>
+          <t>510704654</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Rua António Nobre, Nº 1D, 3º Dtº</t>
+          <t>Rua Comandante Luís Pinto da Silva, Nº 70, R/C, Loja 9</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2800-260 Cacilhas</t>
+          <t>4830-535 Póvoa de Lanhoso</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -3135,14 +3331,20 @@
       <c r="M34" t="n">
         <v>0</v>
       </c>
-      <c r="N34" t="n">
-        <v>0</v>
-      </c>
-      <c r="O34" t="n">
-        <v>0</v>
-      </c>
-      <c r="P34" t="n">
-        <v>0</v>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
@@ -3158,7 +3360,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>748409</t>
+          <t>748482</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3168,35 +3370,31 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ZERO DOSAGE, LDA</t>
+          <t>PARTILHEMPATIA TECNOLOGIA LDA.</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>33</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>ZERO DOSAGE</t>
-        </is>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.racius.com/zero-dosage-lda/</t>
+          <t>https://www.racius.com/partilhempatia-tecnologia-lda/</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>518764230</t>
+          <t>518700330</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Rua Correia de Sá, Nº 349, Casa 7</t>
+          <t>Rua da Prata, Nº 80</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>4150-229 Lordelo do Ouro</t>
+          <t>1100-420 Lisboa</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -3217,14 +3415,20 @@
       <c r="M35" t="n">
         <v>0</v>
       </c>
-      <c r="N35" t="n">
-        <v>0</v>
-      </c>
-      <c r="O35" t="n">
-        <v>0</v>
-      </c>
-      <c r="P35" t="n">
-        <v>0</v>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
@@ -3240,7 +3444,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>748413</t>
+          <t>748489</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3250,35 +3454,35 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TOPPERFORMANCE, LDA</t>
+          <t>INVENIO ENGENHARIA, S.A.</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>SIMPLIFICAMENTE</t>
+          <t>INVENIO - O FUTURO CONSTROI-SE</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.racius.com/topperformance-lda/</t>
+          <t>https://www.racius.com/invenio-engenharia-s-a/</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>510704654</t>
+          <t>510637981</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Rua Comandante Luís Pinto da Silva, Nº 70, R/C, Loja 9</t>
+          <t>Rua Bento Carqueja, Armazém 1, Zona Industrial da Maia, Sector X</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>4830-535 Póvoa de Lanhoso</t>
+          <t>4475-248 Maia</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -3299,14 +3503,20 @@
       <c r="M36" t="n">
         <v>0</v>
       </c>
-      <c r="N36" t="n">
-        <v>0</v>
-      </c>
-      <c r="O36" t="n">
-        <v>0</v>
-      </c>
-      <c r="P36" t="n">
-        <v>0</v>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
@@ -3322,41 +3532,39 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>748482</t>
+          <t>58240</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2025.06.25</t>
+          <t>2025.06.23</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>PARTILHEMPATIA TECNOLOGIA LDA.</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>9</v>
-      </c>
+          <t>TIMBREPIONEIRO, LDA.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.racius.com/partilhempatia-tecnologia-lda/</t>
+          <t>https://www.racius.com/timbrepioneiro-lda/</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>518700330</t>
+          <t>518831051</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Rua da Prata, Nº 80</t>
+          <t>Rua Dr. Dinis Moreira da Mota, Nº. 68 B, 2.º Esqº.</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>1100-420 Lisboa</t>
+          <t>9600-075 Pico da Pedra</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -3377,14 +3585,20 @@
       <c r="M37" t="n">
         <v>0</v>
       </c>
-      <c r="N37" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" t="n">
-        <v>0</v>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>28€</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>6,44€</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>34,44€</t>
+        </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
@@ -3394,246 +3608,6 @@
       <c r="R37" t="inlineStr">
         <is>
           <t>12382</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>748489</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>2025.06.25</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>INVENIO ENGENHARIA, S.A.</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>37</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>INVENIO - O FUTURO CONSTROI-SE</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>https://www.racius.com/invenio-engenharia-s-a/</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>510637981</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Rua Bento Carqueja, Armazém 1, Zona Industrial da Maia, Sector X</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>4475-248 Maia</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>07/2025</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>07/2035</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>2025-07-11</t>
-        </is>
-      </c>
-      <c r="M38" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" t="n">
-        <v>0</v>
-      </c>
-      <c r="P38" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>123456827</t>
-        </is>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>12383</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>748679</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>2025.07.03</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>GOLDENPRAXIS,LDA</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>36</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>C&amp;F REALESTATE art.12º-5 do cpi</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>https://www.racius.com/goldenpraxis-lda/</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>516941925</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Rua Cidade Rio de Janeiro, Nº 25, 5º D - São Marcos</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>2735-659 Agualva-Cacém Sintra</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>07/2025</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>07/2035</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>2025-07-11</t>
-        </is>
-      </c>
-      <c r="M39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" t="n">
-        <v>0</v>
-      </c>
-      <c r="P39" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>123456828</t>
-        </is>
-      </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>12384</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>58240</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>2025.06.23</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>TIMBREPIONEIRO, LDA.</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>https://www.racius.com/timbrepioneiro-lda/</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>518831051</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>Rua Dr. Dinis Moreira da Mota, Nº. 68 B, 2.º Esqº.</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>9600-075 Pico da Pedra</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>07/2025</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>07/2035</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>2025-07-11</t>
-        </is>
-      </c>
-      <c r="M40" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" t="n">
-        <v>0</v>
-      </c>
-      <c r="O40" t="n">
-        <v>0</v>
-      </c>
-      <c r="P40" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>123456829</t>
-        </is>
-      </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>12385</t>
         </is>
       </c>
     </row>

</xml_diff>